<commit_message>
MNT/SM: Add a sheet of data for 20MeV 86Kr17.
</commit_message>
<xml_diff>
--- a/phantasy_apps/settings_manager/contrib/settings_support_cavity_tuning/phase_scan_setting_86Kr17_ver20210709.xlsx
+++ b/phantasy_apps/settings_manager/contrib/settings_support_cavity_tuning/phase_scan_setting_86Kr17_ver20210709.xlsx
@@ -9,6 +9,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="91">
   <si>
     <t xml:space="preserve">[MeV/u]</t>
   </si>
@@ -391,28 +392,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A2:CG10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="37.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="3" style="0" width="12.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="11.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="74" min="12" style="0" width="12.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="75" min="75" style="0" width="10.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="75" min="75" style="0" width="10.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="82" min="76" style="0" width="12.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="83" min="83" style="0" width="9.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="83" min="83" style="0" width="9.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="85" min="84" style="0" width="12.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="86" style="0" width="8.53"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2707,4 +2707,2315 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A2:CG10"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="BW1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.14"/>
+  </cols>
+  <sheetData>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C2" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="M2" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="N2" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="O2" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="P2" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q2" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="R2" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="S2" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="T2" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="U2" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="V2" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="W2" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="X2" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y2" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z2" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA2" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB2" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="AC2" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD2" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="AE2" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF2" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="AG2" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="AH2" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="AI2" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="AJ2" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="AK2" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="AL2" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="AM2" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="AN2" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="AO2" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="AP2" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="AQ2" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="AR2" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="AS2" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="AT2" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="AU2" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="AV2" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="AW2" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="AX2" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="AY2" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="AZ2" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="BA2" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="BB2" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="BC2" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="BD2" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="BE2" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="BF2" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="BG2" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="BH2" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="BI2" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="BJ2" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="BK2" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="BL2" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="BM2" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="BN2" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="BO2" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="BP2" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="BQ2" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="BR2" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="BS2" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="BT2" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="BU2" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="BV2" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="BW2" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="BX2" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="BY2" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="BZ2" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="CA2" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="CB2" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="CC2" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="CD2" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="CE2" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="CF2" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="CG2" s="0" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>95.788581013752</v>
+      </c>
+      <c r="E3" s="1" t="n">
+        <v>106.809754938707</v>
+      </c>
+      <c r="F3" s="1" t="n">
+        <v>103.442481380348</v>
+      </c>
+      <c r="G3" s="1" t="n">
+        <v>79.8495933840465</v>
+      </c>
+      <c r="H3" s="1" t="n">
+        <v>99.5261733534472</v>
+      </c>
+      <c r="I3" s="1" t="n">
+        <v>92.6205163866611</v>
+      </c>
+      <c r="J3" s="1" t="n">
+        <v>70.8190173843644</v>
+      </c>
+      <c r="K3" s="1" t="n">
+        <v>94.9975099017104</v>
+      </c>
+      <c r="L3" s="1" t="n">
+        <v>79.1799044258065</v>
+      </c>
+      <c r="M3" s="1" t="n">
+        <v>19.6859344171111</v>
+      </c>
+      <c r="N3" s="1" t="n">
+        <v>81.5119183548589</v>
+      </c>
+      <c r="O3" s="1" t="n">
+        <v>90.5868189354164</v>
+      </c>
+      <c r="P3" s="1" t="n">
+        <v>37.9035871203964</v>
+      </c>
+      <c r="Q3" s="1" t="n">
+        <v>40.3697283407564</v>
+      </c>
+      <c r="R3" s="1" t="n">
+        <v>36.1091072659646</v>
+      </c>
+      <c r="S3" s="1" t="n">
+        <v>35.7580195430215</v>
+      </c>
+      <c r="T3" s="1" t="n">
+        <v>31.5316574055437</v>
+      </c>
+      <c r="U3" s="1" t="n">
+        <v>29.0594800935079</v>
+      </c>
+      <c r="V3" s="1" t="n">
+        <v>24.1619683153632</v>
+      </c>
+      <c r="W3" s="1" t="n">
+        <v>22.7099112934445</v>
+      </c>
+      <c r="X3" s="1" t="n">
+        <v>23.12399383093</v>
+      </c>
+      <c r="Y3" s="1" t="n">
+        <v>22.3973738783368</v>
+      </c>
+      <c r="Z3" s="1" t="n">
+        <v>20.7480831629341</v>
+      </c>
+      <c r="AA3" s="1" t="n">
+        <v>21.0340033457646</v>
+      </c>
+      <c r="AB3" s="1" t="n">
+        <v>21.0747314394195</v>
+      </c>
+      <c r="AC3" s="1" t="n">
+        <v>18.6358418979482</v>
+      </c>
+      <c r="AD3" s="1" t="n">
+        <v>19.5295857189728</v>
+      </c>
+      <c r="AE3" s="1" t="n">
+        <v>18.8631989130085</v>
+      </c>
+      <c r="AF3" s="1" t="n">
+        <v>17.4220402527517</v>
+      </c>
+      <c r="AG3" s="1" t="n">
+        <v>18.3506966353629</v>
+      </c>
+      <c r="AH3" s="1" t="n">
+        <v>18.0092505134357</v>
+      </c>
+      <c r="AI3" s="1" t="n">
+        <v>15.4500378990957</v>
+      </c>
+      <c r="AJ3" s="1" t="n">
+        <v>17.0825267978849</v>
+      </c>
+      <c r="AK3" s="1" t="n">
+        <v>16.5691482784963</v>
+      </c>
+      <c r="AL3" s="1" t="n">
+        <v>15.5697716161154</v>
+      </c>
+      <c r="AM3" s="1" t="n">
+        <v>16.0198813905457</v>
+      </c>
+      <c r="AN3" s="1" t="n">
+        <v>15.9316792334453</v>
+      </c>
+      <c r="AO3" s="1" t="n">
+        <v>14.0203108665414</v>
+      </c>
+      <c r="AP3" s="1" t="n">
+        <v>15.452346914822</v>
+      </c>
+      <c r="AQ3" s="1" t="n">
+        <v>14.7804926600797</v>
+      </c>
+      <c r="AR3" s="1" t="n">
+        <v>14.0140047849197</v>
+      </c>
+      <c r="AS3" s="1" t="n">
+        <v>14.2757572668065</v>
+      </c>
+      <c r="AT3" s="1" t="n">
+        <v>14.6507523665937</v>
+      </c>
+      <c r="AU3" s="1" t="n">
+        <v>11.8943010865912</v>
+      </c>
+      <c r="AV3" s="1" t="n">
+        <v>14.2046056251575</v>
+      </c>
+      <c r="AW3" s="1" t="n">
+        <v>13.0205633842827</v>
+      </c>
+      <c r="AX3" s="1" t="n">
+        <v>12.2733341223371</v>
+      </c>
+      <c r="AY3" s="1" t="n">
+        <v>13.2549438887887</v>
+      </c>
+      <c r="AZ3" s="1" t="n">
+        <v>12.0031847522136</v>
+      </c>
+      <c r="BA3" s="1" t="n">
+        <v>12.3243536109645</v>
+      </c>
+      <c r="BB3" s="1" t="n">
+        <v>13.2251218049427</v>
+      </c>
+      <c r="BC3" s="1" t="n">
+        <v>11.8783314204427</v>
+      </c>
+      <c r="BD3" s="1" t="n">
+        <v>16.8456336508097</v>
+      </c>
+      <c r="BE3" s="1" t="n">
+        <v>16.1977246642401</v>
+      </c>
+      <c r="BF3" s="1" t="n">
+        <v>10.5825134473035</v>
+      </c>
+      <c r="BG3" s="1" t="n">
+        <v>21.7686702615713</v>
+      </c>
+      <c r="BH3" s="1" t="n">
+        <v>19.052460879646</v>
+      </c>
+      <c r="BI3" s="1" t="n">
+        <v>21.537584853177</v>
+      </c>
+      <c r="BJ3" s="1" t="n">
+        <v>23.9828992726579</v>
+      </c>
+      <c r="BK3" s="1" t="n">
+        <v>25.3462121586354</v>
+      </c>
+      <c r="BL3" s="1" t="n">
+        <v>19.3747726093347</v>
+      </c>
+      <c r="BM3" s="1" t="n">
+        <v>13.8769339880829</v>
+      </c>
+      <c r="BN3" s="1" t="n">
+        <v>11.7889312670427</v>
+      </c>
+      <c r="BO3" s="1" t="n">
+        <v>20.8465765066787</v>
+      </c>
+      <c r="BP3" s="1" t="n">
+        <v>20.8465765066787</v>
+      </c>
+      <c r="BQ3" s="1" t="n">
+        <v>20.8465765066787</v>
+      </c>
+      <c r="BR3" s="1" t="n">
+        <v>20.8465765066787</v>
+      </c>
+      <c r="BS3" s="1" t="n">
+        <v>21.984379750157</v>
+      </c>
+      <c r="BT3" s="1" t="n">
+        <v>23.517879549951</v>
+      </c>
+      <c r="BU3" s="1" t="n">
+        <v>23.8436942345997</v>
+      </c>
+      <c r="BV3" s="1" t="n">
+        <v>0.606326513811193</v>
+      </c>
+      <c r="BW3" s="1" t="n">
+        <v>5.21065385605056E-013</v>
+      </c>
+      <c r="BX3" s="1" t="n">
+        <v>23.2741235669764</v>
+      </c>
+      <c r="BY3" s="1" t="n">
+        <v>23.5804618804817</v>
+      </c>
+      <c r="BZ3" s="1" t="n">
+        <v>21.8544861208573</v>
+      </c>
+      <c r="CA3" s="1" t="n">
+        <v>10.6793559452092</v>
+      </c>
+      <c r="CB3" s="1" t="n">
+        <v>15.2562227788704</v>
+      </c>
+      <c r="CC3" s="1" t="n">
+        <v>15.2562227788704</v>
+      </c>
+      <c r="CD3" s="1" t="n">
+        <v>10.6793559452092</v>
+      </c>
+      <c r="CE3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="CF3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="CG3" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>95.788581013752</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <v>106.809754938707</v>
+      </c>
+      <c r="F4" s="1" t="n">
+        <v>103.442481380348</v>
+      </c>
+      <c r="G4" s="1" t="n">
+        <v>79.8495933840465</v>
+      </c>
+      <c r="H4" s="1" t="n">
+        <v>99.5261733534472</v>
+      </c>
+      <c r="I4" s="1" t="n">
+        <v>92.6205163866611</v>
+      </c>
+      <c r="J4" s="1" t="n">
+        <v>70.8190173843644</v>
+      </c>
+      <c r="K4" s="1" t="n">
+        <v>94.9975099017104</v>
+      </c>
+      <c r="L4" s="1" t="n">
+        <v>79.1799044258065</v>
+      </c>
+      <c r="M4" s="1" t="n">
+        <v>19.6859344171111</v>
+      </c>
+      <c r="N4" s="1" t="n">
+        <v>81.5119183548589</v>
+      </c>
+      <c r="O4" s="1" t="n">
+        <v>90.5868189354164</v>
+      </c>
+      <c r="P4" s="1" t="n">
+        <v>37.9035871203964</v>
+      </c>
+      <c r="Q4" s="1" t="n">
+        <v>40.3697283407564</v>
+      </c>
+      <c r="R4" s="1" t="n">
+        <v>39.9689439664092</v>
+      </c>
+      <c r="S4" s="1" t="n">
+        <v>43.7701728738714</v>
+      </c>
+      <c r="T4" s="1" t="n">
+        <v>38.5968270412695</v>
+      </c>
+      <c r="U4" s="1" t="n">
+        <v>35.5707190603036</v>
+      </c>
+      <c r="V4" s="1" t="n">
+        <v>29.5758418293846</v>
+      </c>
+      <c r="W4" s="1" t="n">
+        <v>27.7984283237057</v>
+      </c>
+      <c r="X4" s="1" t="n">
+        <v>28.305292643414</v>
+      </c>
+      <c r="Y4" s="1" t="n">
+        <v>27.4158619270304</v>
+      </c>
+      <c r="Z4" s="1" t="n">
+        <v>25.3970213800703</v>
+      </c>
+      <c r="AA4" s="1" t="n">
+        <v>25.7470065299906</v>
+      </c>
+      <c r="AB4" s="1" t="n">
+        <v>25.7968604011748</v>
+      </c>
+      <c r="AC4" s="1" t="n">
+        <v>22.8114988455091</v>
+      </c>
+      <c r="AD4" s="1" t="n">
+        <v>23.9055001926514</v>
+      </c>
+      <c r="AE4" s="1" t="n">
+        <v>23.0897988179477</v>
+      </c>
+      <c r="AF4" s="1" t="n">
+        <v>21.3257256252971</v>
+      </c>
+      <c r="AG4" s="1" t="n">
+        <v>22.462462249047</v>
+      </c>
+      <c r="AH4" s="1" t="n">
+        <v>22.0445096897369</v>
+      </c>
+      <c r="AI4" s="1" t="n">
+        <v>18.911864761908</v>
+      </c>
+      <c r="AJ4" s="1" t="n">
+        <v>20.9101387778587</v>
+      </c>
+      <c r="AK4" s="1" t="n">
+        <v>20.281729631308</v>
+      </c>
+      <c r="AL4" s="1" t="n">
+        <v>19.0584267236653</v>
+      </c>
+      <c r="AM4" s="1" t="n">
+        <v>19.6093907560925</v>
+      </c>
+      <c r="AN4" s="1" t="n">
+        <v>19.5014255020468</v>
+      </c>
+      <c r="AO4" s="1" t="n">
+        <v>17.1617846350693</v>
+      </c>
+      <c r="AP4" s="1" t="n">
+        <v>18.9146911493533</v>
+      </c>
+      <c r="AQ4" s="1" t="n">
+        <v>18.0922972569641</v>
+      </c>
+      <c r="AR4" s="1" t="n">
+        <v>17.1540655755054</v>
+      </c>
+      <c r="AS4" s="1" t="n">
+        <v>17.4744678664814</v>
+      </c>
+      <c r="AT4" s="1" t="n">
+        <v>17.9334865860387</v>
+      </c>
+      <c r="AU4" s="1" t="n">
+        <v>14.5594085306543</v>
+      </c>
+      <c r="AV4" s="1" t="n">
+        <v>17.3873735672156</v>
+      </c>
+      <c r="AW4" s="1" t="n">
+        <v>15.9380278194539</v>
+      </c>
+      <c r="AX4" s="1" t="n">
+        <v>15.0233699499815</v>
+      </c>
+      <c r="AY4" s="1" t="n">
+        <v>16.22492500592</v>
+      </c>
+      <c r="AZ4" s="1" t="n">
+        <v>14.6926893143315</v>
+      </c>
+      <c r="BA4" s="1" t="n">
+        <v>15.0858211669587</v>
+      </c>
+      <c r="BB4" s="1" t="n">
+        <v>16.1884208096004</v>
+      </c>
+      <c r="BC4" s="1" t="n">
+        <v>14.5461183827588</v>
+      </c>
+      <c r="BD4" s="1" t="n">
+        <v>20.6290406155488</v>
+      </c>
+      <c r="BE4" s="1" t="n">
+        <v>19.8356159764892</v>
+      </c>
+      <c r="BF4" s="1" t="n">
+        <v>12.9592691046396</v>
+      </c>
+      <c r="BG4" s="1" t="n">
+        <v>26.6577554920803</v>
+      </c>
+      <c r="BH4" s="1" t="n">
+        <v>23.3315052113508</v>
+      </c>
+      <c r="BI4" s="1" t="n">
+        <v>26.3747699793805</v>
+      </c>
+      <c r="BJ4" s="1" t="n">
+        <v>29.3692842566653</v>
+      </c>
+      <c r="BK4" s="1" t="n">
+        <v>31.038787314817</v>
+      </c>
+      <c r="BL4" s="1" t="n">
+        <v>23.7262058145125</v>
+      </c>
+      <c r="BM4" s="1" t="n">
+        <v>16.9935925708376</v>
+      </c>
+      <c r="BN4" s="1" t="n">
+        <v>14.4366396042364</v>
+      </c>
+      <c r="BO4" s="1" t="n">
+        <v>26.4737159785725</v>
+      </c>
+      <c r="BP4" s="1" t="n">
+        <v>26.4737159785725</v>
+      </c>
+      <c r="BQ4" s="1" t="n">
+        <v>26.4737159785725</v>
+      </c>
+      <c r="BR4" s="1" t="n">
+        <v>26.4737159785725</v>
+      </c>
+      <c r="BS4" s="1" t="n">
+        <v>26.9219117650609</v>
+      </c>
+      <c r="BT4" s="1" t="n">
+        <v>28.7998244817704</v>
+      </c>
+      <c r="BU4" s="1" t="n">
+        <v>29.1988147781335</v>
+      </c>
+      <c r="BV4" s="1" t="n">
+        <v>0.742503044941502</v>
+      </c>
+      <c r="BW4" s="1" t="n">
+        <v>6.38092886609027E-013</v>
+      </c>
+      <c r="BX4" s="1" t="n">
+        <v>28.5013226754686</v>
+      </c>
+      <c r="BY4" s="1" t="n">
+        <v>28.8764623491903</v>
+      </c>
+      <c r="BZ4" s="1" t="n">
+        <v>26.762844970064</v>
+      </c>
+      <c r="CA4" s="1" t="n">
+        <v>13.0778617241884</v>
+      </c>
+      <c r="CB4" s="1" t="n">
+        <v>18.6826596059835</v>
+      </c>
+      <c r="CC4" s="1" t="n">
+        <v>18.6826596059835</v>
+      </c>
+      <c r="CD4" s="1" t="n">
+        <v>13.0778617241884</v>
+      </c>
+      <c r="CE4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="CF4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="CG4" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>95.788581013752</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <v>106.809754938707</v>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>103.442481380348</v>
+      </c>
+      <c r="G5" s="1" t="n">
+        <v>79.8495933840465</v>
+      </c>
+      <c r="H5" s="1" t="n">
+        <v>99.5261733534472</v>
+      </c>
+      <c r="I5" s="1" t="n">
+        <v>92.6205163866611</v>
+      </c>
+      <c r="J5" s="1" t="n">
+        <v>70.8190173843644</v>
+      </c>
+      <c r="K5" s="1" t="n">
+        <v>94.9975099017104</v>
+      </c>
+      <c r="L5" s="1" t="n">
+        <v>79.1799044258065</v>
+      </c>
+      <c r="M5" s="1" t="n">
+        <v>19.6859344171111</v>
+      </c>
+      <c r="N5" s="1" t="n">
+        <v>81.5119183548589</v>
+      </c>
+      <c r="O5" s="1" t="n">
+        <v>90.5868189354164</v>
+      </c>
+      <c r="P5" s="1" t="n">
+        <v>37.9035871203964</v>
+      </c>
+      <c r="Q5" s="1" t="n">
+        <v>40.3697283407564</v>
+      </c>
+      <c r="R5" s="1" t="n">
+        <v>39.9689439664092</v>
+      </c>
+      <c r="S5" s="1" t="n">
+        <v>43.7701728738714</v>
+      </c>
+      <c r="T5" s="1" t="n">
+        <v>42.2053190283762</v>
+      </c>
+      <c r="U5" s="1" t="n">
+        <v>42.0504065027361</v>
+      </c>
+      <c r="V5" s="1" t="n">
+        <v>34.9634813251266</v>
+      </c>
+      <c r="W5" s="1" t="n">
+        <v>32.8622879162853</v>
+      </c>
+      <c r="X5" s="1" t="n">
+        <v>33.4614844253391</v>
+      </c>
+      <c r="Y5" s="1" t="n">
+        <v>32.4100318776259</v>
+      </c>
+      <c r="Z5" s="1" t="n">
+        <v>30.0234322275046</v>
+      </c>
+      <c r="AA5" s="1" t="n">
+        <v>30.437171904769</v>
+      </c>
+      <c r="AB5" s="1" t="n">
+        <v>30.4961073326831</v>
+      </c>
+      <c r="AC5" s="1" t="n">
+        <v>26.9669218034122</v>
+      </c>
+      <c r="AD5" s="1" t="n">
+        <v>28.2602102883563</v>
+      </c>
+      <c r="AE5" s="1" t="n">
+        <v>27.2959178788332</v>
+      </c>
+      <c r="AF5" s="1" t="n">
+        <v>25.210494901418</v>
+      </c>
+      <c r="AG5" s="1" t="n">
+        <v>26.5543034714443</v>
+      </c>
+      <c r="AH5" s="1" t="n">
+        <v>26.0602152021559</v>
+      </c>
+      <c r="AI5" s="1" t="n">
+        <v>22.3569166430062</v>
+      </c>
+      <c r="AJ5" s="1" t="n">
+        <v>24.7192032904065</v>
+      </c>
+      <c r="AK5" s="1" t="n">
+        <v>23.9763209208459</v>
+      </c>
+      <c r="AL5" s="1" t="n">
+        <v>22.5301768478192</v>
+      </c>
+      <c r="AM5" s="1" t="n">
+        <v>23.1815064285531</v>
+      </c>
+      <c r="AN5" s="1" t="n">
+        <v>23.0538738436426</v>
+      </c>
+      <c r="AO5" s="1" t="n">
+        <v>20.2880357575463</v>
+      </c>
+      <c r="AP5" s="1" t="n">
+        <v>22.3602578951414</v>
+      </c>
+      <c r="AQ5" s="1" t="n">
+        <v>21.3880538353442</v>
+      </c>
+      <c r="AR5" s="1" t="n">
+        <v>20.2789105669104</v>
+      </c>
+      <c r="AS5" s="1" t="n">
+        <v>20.6576784674724</v>
+      </c>
+      <c r="AT5" s="1" t="n">
+        <v>21.2003136533686</v>
+      </c>
+      <c r="AU5" s="1" t="n">
+        <v>17.2116016579675</v>
+      </c>
+      <c r="AV5" s="1" t="n">
+        <v>20.5547187639592</v>
+      </c>
+      <c r="AW5" s="1" t="n">
+        <v>18.8413550910723</v>
+      </c>
+      <c r="AX5" s="1" t="n">
+        <v>17.7600799232289</v>
+      </c>
+      <c r="AY5" s="1" t="n">
+        <v>19.1805144793022</v>
+      </c>
+      <c r="AZ5" s="1" t="n">
+        <v>17.369161338533</v>
+      </c>
+      <c r="BA5" s="1" t="n">
+        <v>17.8339074738058</v>
+      </c>
+      <c r="BB5" s="1" t="n">
+        <v>19.1373605500354</v>
+      </c>
+      <c r="BC5" s="1" t="n">
+        <v>17.1907786416449</v>
+      </c>
+      <c r="BD5" s="1" t="n">
+        <v>24.3796497099691</v>
+      </c>
+      <c r="BE5" s="1" t="n">
+        <v>23.4419708749703</v>
+      </c>
+      <c r="BF5" s="1" t="n">
+        <v>15.3154209716473</v>
+      </c>
+      <c r="BG5" s="1" t="n">
+        <v>31.5044578690231</v>
+      </c>
+      <c r="BH5" s="1" t="n">
+        <v>27.5734550558942</v>
+      </c>
+      <c r="BI5" s="1" t="n">
+        <v>31.1700221673736</v>
+      </c>
+      <c r="BJ5" s="1" t="n">
+        <v>34.7089753592482</v>
+      </c>
+      <c r="BK5" s="1" t="n">
+        <v>36.6820142661948</v>
+      </c>
+      <c r="BL5" s="1" t="n">
+        <v>28.039917002658</v>
+      </c>
+      <c r="BM5" s="1" t="n">
+        <v>20.0832332395858</v>
+      </c>
+      <c r="BN5" s="1" t="n">
+        <v>17.0613952970294</v>
+      </c>
+      <c r="BO5" s="1" t="n">
+        <v>32.0132208750451</v>
+      </c>
+      <c r="BP5" s="1" t="n">
+        <v>32.0132208750451</v>
+      </c>
+      <c r="BQ5" s="1" t="n">
+        <v>32.0132208750451</v>
+      </c>
+      <c r="BR5" s="1" t="n">
+        <v>32.0132208750451</v>
+      </c>
+      <c r="BS5" s="1" t="n">
+        <v>31.8166409474307</v>
+      </c>
+      <c r="BT5" s="1" t="n">
+        <v>34.0359809095987</v>
+      </c>
+      <c r="BU5" s="1" t="n">
+        <v>34.5075124676721</v>
+      </c>
+      <c r="BV5" s="1" t="n">
+        <v>0.877499079167803</v>
+      </c>
+      <c r="BW5" s="1" t="n">
+        <v>7.54105891198143E-013</v>
+      </c>
+      <c r="BX5" s="1" t="n">
+        <v>33.6832078644991</v>
+      </c>
+      <c r="BY5" s="1" t="n">
+        <v>34.126552468259</v>
+      </c>
+      <c r="BZ5" s="1" t="n">
+        <v>31.6286538851731</v>
+      </c>
+      <c r="CA5" s="1" t="n">
+        <v>15.4555751638208</v>
+      </c>
+      <c r="CB5" s="1" t="n">
+        <v>22.0793930911726</v>
+      </c>
+      <c r="CC5" s="1" t="n">
+        <v>22.0793930911726</v>
+      </c>
+      <c r="CD5" s="1" t="n">
+        <v>15.4555751638208</v>
+      </c>
+      <c r="CE5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="CF5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="CG5" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>95.788581013752</v>
+      </c>
+      <c r="E6" s="1" t="n">
+        <v>106.809754938707</v>
+      </c>
+      <c r="F6" s="1" t="n">
+        <v>103.442481380348</v>
+      </c>
+      <c r="G6" s="1" t="n">
+        <v>79.8495933840465</v>
+      </c>
+      <c r="H6" s="1" t="n">
+        <v>99.5261733534472</v>
+      </c>
+      <c r="I6" s="1" t="n">
+        <v>92.6205163866611</v>
+      </c>
+      <c r="J6" s="1" t="n">
+        <v>70.8190173843644</v>
+      </c>
+      <c r="K6" s="1" t="n">
+        <v>94.9975099017104</v>
+      </c>
+      <c r="L6" s="1" t="n">
+        <v>79.1799044258065</v>
+      </c>
+      <c r="M6" s="1" t="n">
+        <v>19.6859344171111</v>
+      </c>
+      <c r="N6" s="1" t="n">
+        <v>81.5119183548589</v>
+      </c>
+      <c r="O6" s="1" t="n">
+        <v>90.5868189354164</v>
+      </c>
+      <c r="P6" s="1" t="n">
+        <v>37.9035871203964</v>
+      </c>
+      <c r="Q6" s="1" t="n">
+        <v>40.3697283407564</v>
+      </c>
+      <c r="R6" s="1" t="n">
+        <v>39.9689439664092</v>
+      </c>
+      <c r="S6" s="1" t="n">
+        <v>43.7701728738714</v>
+      </c>
+      <c r="T6" s="1" t="n">
+        <v>42.2053190283762</v>
+      </c>
+      <c r="U6" s="1" t="n">
+        <v>42.0504065027361</v>
+      </c>
+      <c r="V6" s="1" t="n">
+        <v>37.5261607005142</v>
+      </c>
+      <c r="W6" s="1" t="n">
+        <v>39.808866914046</v>
+      </c>
+      <c r="X6" s="1" t="n">
+        <v>45.5398127012069</v>
+      </c>
+      <c r="Y6" s="1" t="n">
+        <v>44.1088256153259</v>
+      </c>
+      <c r="Z6" s="1" t="n">
+        <v>40.8607539016578</v>
+      </c>
+      <c r="AA6" s="1" t="n">
+        <v>41.4238379289585</v>
+      </c>
+      <c r="AB6" s="1" t="n">
+        <v>41.5040468137335</v>
+      </c>
+      <c r="AC6" s="1" t="n">
+        <v>36.7009590024498</v>
+      </c>
+      <c r="AD6" s="1" t="n">
+        <v>38.4610756375738</v>
+      </c>
+      <c r="AE6" s="1" t="n">
+        <v>37.1487101979334</v>
+      </c>
+      <c r="AF6" s="1" t="n">
+        <v>34.3105285265201</v>
+      </c>
+      <c r="AG6" s="1" t="n">
+        <v>36.1394010836184</v>
+      </c>
+      <c r="AH6" s="1" t="n">
+        <v>35.4669656663713</v>
+      </c>
+      <c r="AI6" s="1" t="n">
+        <v>30.4269166172439</v>
+      </c>
+      <c r="AJ6" s="1" t="n">
+        <v>33.6418992552438</v>
+      </c>
+      <c r="AK6" s="1" t="n">
+        <v>32.6308644924465</v>
+      </c>
+      <c r="AL6" s="1" t="n">
+        <v>30.6627171924802</v>
+      </c>
+      <c r="AM6" s="1" t="n">
+        <v>31.5491520779246</v>
+      </c>
+      <c r="AN6" s="1" t="n">
+        <v>31.3754489648914</v>
+      </c>
+      <c r="AO6" s="1" t="n">
+        <v>27.6112481063274</v>
+      </c>
+      <c r="AP6" s="1" t="n">
+        <v>30.4314639348252</v>
+      </c>
+      <c r="AQ6" s="1" t="n">
+        <v>29.1083310388741</v>
+      </c>
+      <c r="AR6" s="1" t="n">
+        <v>27.5988290675561</v>
+      </c>
+      <c r="AS6" s="1" t="n">
+        <v>28.1143178315799</v>
+      </c>
+      <c r="AT6" s="1" t="n">
+        <v>28.852823763256</v>
+      </c>
+      <c r="AU6" s="1" t="n">
+        <v>23.4243378395392</v>
+      </c>
+      <c r="AV6" s="1" t="n">
+        <v>27.9741935754603</v>
+      </c>
+      <c r="AW6" s="1" t="n">
+        <v>25.6423705230067</v>
+      </c>
+      <c r="AX6" s="1" t="n">
+        <v>24.1707959808812</v>
+      </c>
+      <c r="AY6" s="1" t="n">
+        <v>26.1039536022124</v>
+      </c>
+      <c r="AZ6" s="1" t="n">
+        <v>23.6387705960483</v>
+      </c>
+      <c r="BA6" s="1" t="n">
+        <v>24.2712724804509</v>
+      </c>
+      <c r="BB6" s="1" t="n">
+        <v>26.0452227392553</v>
+      </c>
+      <c r="BC6" s="1" t="n">
+        <v>23.3951519555293</v>
+      </c>
+      <c r="BD6" s="1" t="n">
+        <v>33.1785791369325</v>
+      </c>
+      <c r="BE6" s="1" t="n">
+        <v>31.9024799393581</v>
+      </c>
+      <c r="BF6" s="1" t="n">
+        <v>20.8429535603806</v>
+      </c>
+      <c r="BG6" s="1" t="n">
+        <v>42.8748222804084</v>
+      </c>
+      <c r="BH6" s="1" t="n">
+        <v>37.5250699470282</v>
+      </c>
+      <c r="BI6" s="1" t="n">
+        <v>42.4196844287412</v>
+      </c>
+      <c r="BJ6" s="1" t="n">
+        <v>47.2358913855826</v>
+      </c>
+      <c r="BK6" s="1" t="n">
+        <v>49.9210254335754</v>
+      </c>
+      <c r="BL6" s="1" t="n">
+        <v>38.1598840152853</v>
+      </c>
+      <c r="BM6" s="1" t="n">
+        <v>27.3315306533136</v>
+      </c>
+      <c r="BN6" s="1" t="n">
+        <v>23.2190724962509</v>
+      </c>
+      <c r="BO6" s="1" t="n">
+        <v>37.1458932600404</v>
+      </c>
+      <c r="BP6" s="1" t="n">
+        <v>37.1458932600404</v>
+      </c>
+      <c r="BQ6" s="1" t="n">
+        <v>37.1458932600404</v>
+      </c>
+      <c r="BR6" s="1" t="n">
+        <v>37.1458932600404</v>
+      </c>
+      <c r="BS6" s="1" t="n">
+        <v>43.2996762506409</v>
+      </c>
+      <c r="BT6" s="1" t="n">
+        <v>46.3200045753927</v>
+      </c>
+      <c r="BU6" s="1" t="n">
+        <v>46.9617179429438</v>
+      </c>
+      <c r="BV6" s="1" t="n">
+        <v>1.19419979315162</v>
+      </c>
+      <c r="BW6" s="1" t="n">
+        <v>1.02627241516573E-012</v>
+      </c>
+      <c r="BX6" s="1" t="n">
+        <v>45.8399111969621</v>
+      </c>
+      <c r="BY6" s="1" t="n">
+        <v>46.4432645755287</v>
+      </c>
+      <c r="BZ6" s="1" t="n">
+        <v>43.0438422375999</v>
+      </c>
+      <c r="CA6" s="1" t="n">
+        <v>21.0336912047571</v>
+      </c>
+      <c r="CB6" s="1" t="n">
+        <v>30.0481302925101</v>
+      </c>
+      <c r="CC6" s="1" t="n">
+        <v>30.0481302925101</v>
+      </c>
+      <c r="CD6" s="1" t="n">
+        <v>21.0336912047571</v>
+      </c>
+      <c r="CE6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="CF6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="CG6" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>95.788581013752</v>
+      </c>
+      <c r="E7" s="1" t="n">
+        <v>106.809754938707</v>
+      </c>
+      <c r="F7" s="1" t="n">
+        <v>103.442481380348</v>
+      </c>
+      <c r="G7" s="1" t="n">
+        <v>79.8495933840465</v>
+      </c>
+      <c r="H7" s="1" t="n">
+        <v>99.5261733534472</v>
+      </c>
+      <c r="I7" s="1" t="n">
+        <v>92.6205163866611</v>
+      </c>
+      <c r="J7" s="1" t="n">
+        <v>70.8190173843644</v>
+      </c>
+      <c r="K7" s="1" t="n">
+        <v>94.9975099017104</v>
+      </c>
+      <c r="L7" s="1" t="n">
+        <v>79.1799044258065</v>
+      </c>
+      <c r="M7" s="1" t="n">
+        <v>19.6859344171111</v>
+      </c>
+      <c r="N7" s="1" t="n">
+        <v>81.5119183548589</v>
+      </c>
+      <c r="O7" s="1" t="n">
+        <v>90.5868189354164</v>
+      </c>
+      <c r="P7" s="1" t="n">
+        <v>37.9035871203964</v>
+      </c>
+      <c r="Q7" s="1" t="n">
+        <v>40.3697283407564</v>
+      </c>
+      <c r="R7" s="1" t="n">
+        <v>39.9689439664092</v>
+      </c>
+      <c r="S7" s="1" t="n">
+        <v>43.7701728738714</v>
+      </c>
+      <c r="T7" s="1" t="n">
+        <v>42.2053190283762</v>
+      </c>
+      <c r="U7" s="1" t="n">
+        <v>42.0504065027361</v>
+      </c>
+      <c r="V7" s="1" t="n">
+        <v>37.5261607005142</v>
+      </c>
+      <c r="W7" s="1" t="n">
+        <v>39.808866914046</v>
+      </c>
+      <c r="X7" s="1" t="n">
+        <v>45.5398127012069</v>
+      </c>
+      <c r="Y7" s="1" t="n">
+        <v>46.5786397293642</v>
+      </c>
+      <c r="Z7" s="1" t="n">
+        <v>48.097119142325</v>
+      </c>
+      <c r="AA7" s="1" t="n">
+        <v>53.9553141671841</v>
+      </c>
+      <c r="AB7" s="1" t="n">
+        <v>54.0597877213839</v>
+      </c>
+      <c r="AC7" s="1" t="n">
+        <v>47.8036771148577</v>
+      </c>
+      <c r="AD7" s="1" t="n">
+        <v>50.0962615485325</v>
+      </c>
+      <c r="AE7" s="1" t="n">
+        <v>48.3868813187386</v>
+      </c>
+      <c r="AF7" s="1" t="n">
+        <v>44.6900972591042</v>
+      </c>
+      <c r="AG7" s="1" t="n">
+        <v>47.0722375513487</v>
+      </c>
+      <c r="AH7" s="1" t="n">
+        <v>46.1963779978007</v>
+      </c>
+      <c r="AI7" s="1" t="n">
+        <v>39.6316210013568</v>
+      </c>
+      <c r="AJ7" s="1" t="n">
+        <v>43.8191952809979</v>
+      </c>
+      <c r="AK7" s="1" t="n">
+        <v>42.5023038245802</v>
+      </c>
+      <c r="AL7" s="1" t="n">
+        <v>39.938755606786</v>
+      </c>
+      <c r="AM7" s="1" t="n">
+        <v>41.0933534210912</v>
+      </c>
+      <c r="AN7" s="1" t="n">
+        <v>40.867101907371</v>
+      </c>
+      <c r="AO7" s="1" t="n">
+        <v>35.964160749178</v>
+      </c>
+      <c r="AP7" s="1" t="n">
+        <v>39.6375439665137</v>
+      </c>
+      <c r="AQ7" s="1" t="n">
+        <v>37.9141389259568</v>
+      </c>
+      <c r="AR7" s="1" t="n">
+        <v>35.947984721749</v>
+      </c>
+      <c r="AS7" s="1" t="n">
+        <v>36.6194183600385</v>
+      </c>
+      <c r="AT7" s="1" t="n">
+        <v>37.5813359792182</v>
+      </c>
+      <c r="AU7" s="1" t="n">
+        <v>30.510632777632</v>
+      </c>
+      <c r="AV7" s="1" t="n">
+        <v>36.4369039277847</v>
+      </c>
+      <c r="AW7" s="1" t="n">
+        <v>33.3996613238235</v>
+      </c>
+      <c r="AX7" s="1" t="n">
+        <v>31.4829082968109</v>
+      </c>
+      <c r="AY7" s="1" t="n">
+        <v>34.000881811783</v>
+      </c>
+      <c r="AZ7" s="1" t="n">
+        <v>30.7899354044197</v>
+      </c>
+      <c r="BA7" s="1" t="n">
+        <v>31.613780793705</v>
+      </c>
+      <c r="BB7" s="1" t="n">
+        <v>33.9243837777863</v>
+      </c>
+      <c r="BC7" s="1" t="n">
+        <v>30.4761738656312</v>
+      </c>
+      <c r="BD7" s="1" t="n">
+        <v>43.2207556639861</v>
+      </c>
+      <c r="BE7" s="1" t="n">
+        <v>41.5584189076789</v>
+      </c>
+      <c r="BF7" s="1" t="n">
+        <v>27.1515003530169</v>
+      </c>
+      <c r="BG7" s="1" t="n">
+        <v>55.8517653896641</v>
+      </c>
+      <c r="BH7" s="1" t="n">
+        <v>48.882800940958</v>
+      </c>
+      <c r="BI7" s="1" t="n">
+        <v>55.2588707452265</v>
+      </c>
+      <c r="BJ7" s="1" t="n">
+        <v>61.5328013813073</v>
+      </c>
+      <c r="BK7" s="1" t="n">
+        <v>65.0306462448374</v>
+      </c>
+      <c r="BL7" s="1" t="n">
+        <v>49.7097544889976</v>
+      </c>
+      <c r="BM7" s="1" t="n">
+        <v>35.6039781997376</v>
+      </c>
+      <c r="BN7" s="1" t="n">
+        <v>30.2468003516085</v>
+      </c>
+      <c r="BO7" s="1" t="n">
+        <v>49.7391872504227</v>
+      </c>
+      <c r="BP7" s="1" t="n">
+        <v>49.7391872504227</v>
+      </c>
+      <c r="BQ7" s="1" t="n">
+        <v>49.7391872504227</v>
+      </c>
+      <c r="BR7" s="1" t="n">
+        <v>49.7391872504227</v>
+      </c>
+      <c r="BS7" s="1" t="n">
+        <v>56.4052101156877</v>
+      </c>
+      <c r="BT7" s="1" t="n">
+        <v>60.3397026691619</v>
+      </c>
+      <c r="BU7" s="1" t="n">
+        <v>61.1756437307357</v>
+      </c>
+      <c r="BV7" s="1" t="n">
+        <v>1.55564881970292</v>
+      </c>
+      <c r="BW7" s="1" t="n">
+        <v>1.33689478134379E-012</v>
+      </c>
+      <c r="BX7" s="1" t="n">
+        <v>59.7142991966562</v>
+      </c>
+      <c r="BY7" s="1" t="n">
+        <v>60.5002698329043</v>
+      </c>
+      <c r="BZ7" s="1" t="n">
+        <v>56.0719426987033</v>
+      </c>
+      <c r="CA7" s="1" t="n">
+        <v>27.399968652081</v>
+      </c>
+      <c r="CB7" s="1" t="n">
+        <v>39.1428123601157</v>
+      </c>
+      <c r="CC7" s="1" t="n">
+        <v>39.1428123601157</v>
+      </c>
+      <c r="CD7" s="1" t="n">
+        <v>27.399968652081</v>
+      </c>
+      <c r="CE7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="CF7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="CG7" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>95.788581013752</v>
+      </c>
+      <c r="E8" s="1" t="n">
+        <v>106.809754938707</v>
+      </c>
+      <c r="F8" s="1" t="n">
+        <v>103.442481380348</v>
+      </c>
+      <c r="G8" s="1" t="n">
+        <v>79.8495933840465</v>
+      </c>
+      <c r="H8" s="1" t="n">
+        <v>99.5261733534472</v>
+      </c>
+      <c r="I8" s="1" t="n">
+        <v>92.6205163866611</v>
+      </c>
+      <c r="J8" s="1" t="n">
+        <v>70.8190173843644</v>
+      </c>
+      <c r="K8" s="1" t="n">
+        <v>94.9975099017104</v>
+      </c>
+      <c r="L8" s="1" t="n">
+        <v>79.1799044258065</v>
+      </c>
+      <c r="M8" s="1" t="n">
+        <v>19.6859344171111</v>
+      </c>
+      <c r="N8" s="1" t="n">
+        <v>81.5119183548589</v>
+      </c>
+      <c r="O8" s="1" t="n">
+        <v>90.5868189354164</v>
+      </c>
+      <c r="P8" s="1" t="n">
+        <v>37.9035871203964</v>
+      </c>
+      <c r="Q8" s="1" t="n">
+        <v>40.3697283407564</v>
+      </c>
+      <c r="R8" s="1" t="n">
+        <v>39.9689439664092</v>
+      </c>
+      <c r="S8" s="1" t="n">
+        <v>43.7701728738714</v>
+      </c>
+      <c r="T8" s="1" t="n">
+        <v>42.2053190283762</v>
+      </c>
+      <c r="U8" s="1" t="n">
+        <v>42.0504065027361</v>
+      </c>
+      <c r="V8" s="1" t="n">
+        <v>37.5261607005142</v>
+      </c>
+      <c r="W8" s="1" t="n">
+        <v>39.808866914046</v>
+      </c>
+      <c r="X8" s="1" t="n">
+        <v>45.5398127012069</v>
+      </c>
+      <c r="Y8" s="1" t="n">
+        <v>46.5786397293642</v>
+      </c>
+      <c r="Z8" s="1" t="n">
+        <v>48.097119142325</v>
+      </c>
+      <c r="AA8" s="1" t="n">
+        <v>53.9553141671841</v>
+      </c>
+      <c r="AB8" s="1" t="n">
+        <v>56.8369813374168</v>
+      </c>
+      <c r="AC8" s="1" t="n">
+        <v>54.6554031688876</v>
+      </c>
+      <c r="AD8" s="1" t="n">
+        <v>61.413465323765</v>
+      </c>
+      <c r="AE8" s="1" t="n">
+        <v>60.8471218490168</v>
+      </c>
+      <c r="AF8" s="1" t="n">
+        <v>59.4342022837237</v>
+      </c>
+      <c r="AG8" s="1" t="n">
+        <v>65.7441311322412</v>
+      </c>
+      <c r="AH8" s="1" t="n">
+        <v>64.5208490377991</v>
+      </c>
+      <c r="AI8" s="1" t="n">
+        <v>55.3520848728345</v>
+      </c>
+      <c r="AJ8" s="1" t="n">
+        <v>61.2007219227815</v>
+      </c>
+      <c r="AK8" s="1" t="n">
+        <v>59.3614661511984</v>
+      </c>
+      <c r="AL8" s="1" t="n">
+        <v>55.7810489252138</v>
+      </c>
+      <c r="AM8" s="1" t="n">
+        <v>57.3936349006707</v>
+      </c>
+      <c r="AN8" s="1" t="n">
+        <v>57.0776374048928</v>
+      </c>
+      <c r="AO8" s="1" t="n">
+        <v>50.2298727094866</v>
+      </c>
+      <c r="AP8" s="1" t="n">
+        <v>55.3603572690116</v>
+      </c>
+      <c r="AQ8" s="1" t="n">
+        <v>52.9533383365307</v>
+      </c>
+      <c r="AR8" s="1" t="n">
+        <v>50.2072802234732</v>
+      </c>
+      <c r="AS8" s="1" t="n">
+        <v>51.1450478644135</v>
+      </c>
+      <c r="AT8" s="1" t="n">
+        <v>52.4885242187036</v>
+      </c>
+      <c r="AU8" s="1" t="n">
+        <v>42.613122864027</v>
+      </c>
+      <c r="AV8" s="1" t="n">
+        <v>50.8901364050945</v>
+      </c>
+      <c r="AW8" s="1" t="n">
+        <v>46.6481269655085</v>
+      </c>
+      <c r="AX8" s="1" t="n">
+        <v>43.9710657313029</v>
+      </c>
+      <c r="AY8" s="1" t="n">
+        <v>47.4878303800037</v>
+      </c>
+      <c r="AZ8" s="1" t="n">
+        <v>43.0032149751378</v>
+      </c>
+      <c r="BA8" s="1" t="n">
+        <v>44.1538507240075</v>
+      </c>
+      <c r="BB8" s="1" t="n">
+        <v>47.3809882785857</v>
+      </c>
+      <c r="BC8" s="1" t="n">
+        <v>42.5646043917936</v>
+      </c>
+      <c r="BD8" s="1" t="n">
+        <v>60.3643480465436</v>
+      </c>
+      <c r="BE8" s="1" t="n">
+        <v>58.0426423524458</v>
+      </c>
+      <c r="BF8" s="1" t="n">
+        <v>37.9211930035979</v>
+      </c>
+      <c r="BG8" s="1" t="n">
+        <v>78.0054710566958</v>
+      </c>
+      <c r="BH8" s="1" t="n">
+        <v>68.2722540168044</v>
+      </c>
+      <c r="BI8" s="1" t="n">
+        <v>77.1774036589388</v>
+      </c>
+      <c r="BJ8" s="1" t="n">
+        <v>85.9399004435988</v>
+      </c>
+      <c r="BK8" s="1" t="n">
+        <v>90.8251719181761</v>
+      </c>
+      <c r="BL8" s="1" t="n">
+        <v>69.4272202136075</v>
+      </c>
+      <c r="BM8" s="1" t="n">
+        <v>49.7263617646869</v>
+      </c>
+      <c r="BN8" s="1" t="n">
+        <v>42.2442494507378</v>
+      </c>
+      <c r="BO8" s="1" t="n">
+        <v>64.5027065275567</v>
+      </c>
+      <c r="BP8" s="1" t="n">
+        <v>64.5027065275567</v>
+      </c>
+      <c r="BQ8" s="1" t="n">
+        <v>64.5027065275567</v>
+      </c>
+      <c r="BR8" s="1" t="n">
+        <v>64.5027065275567</v>
+      </c>
+      <c r="BS8" s="1" t="n">
+        <v>78.7784406532003</v>
+      </c>
+      <c r="BT8" s="1" t="n">
+        <v>84.2735569286048</v>
+      </c>
+      <c r="BU8" s="1" t="n">
+        <v>85.4410755527478</v>
+      </c>
+      <c r="BV8" s="1" t="n">
+        <v>2.17269979083197</v>
+      </c>
+      <c r="BW8" s="1" t="n">
+        <v>1.86717656003152E-012</v>
+      </c>
+      <c r="BX8" s="1" t="n">
+        <v>83.4000860162183</v>
+      </c>
+      <c r="BY8" s="1" t="n">
+        <v>84.4978133537434</v>
+      </c>
+      <c r="BZ8" s="1" t="n">
+        <v>78.3129821011143</v>
+      </c>
+      <c r="CA8" s="1" t="n">
+        <v>38.2682167113703</v>
+      </c>
+      <c r="CB8" s="1" t="n">
+        <v>54.6688810162432</v>
+      </c>
+      <c r="CC8" s="1" t="n">
+        <v>54.6688810162432</v>
+      </c>
+      <c r="CD8" s="1" t="n">
+        <v>38.2682167113703</v>
+      </c>
+      <c r="CE8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="CF8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="CG8" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>95.788581013752</v>
+      </c>
+      <c r="E9" s="1" t="n">
+        <v>106.809754938707</v>
+      </c>
+      <c r="F9" s="1" t="n">
+        <v>103.442481380348</v>
+      </c>
+      <c r="G9" s="1" t="n">
+        <v>79.8495933840465</v>
+      </c>
+      <c r="H9" s="1" t="n">
+        <v>99.5261733534472</v>
+      </c>
+      <c r="I9" s="1" t="n">
+        <v>92.6205163866611</v>
+      </c>
+      <c r="J9" s="1" t="n">
+        <v>70.8190173843644</v>
+      </c>
+      <c r="K9" s="1" t="n">
+        <v>94.9975099017104</v>
+      </c>
+      <c r="L9" s="1" t="n">
+        <v>79.1799044258065</v>
+      </c>
+      <c r="M9" s="1" t="n">
+        <v>19.6859344171111</v>
+      </c>
+      <c r="N9" s="1" t="n">
+        <v>81.5119183548589</v>
+      </c>
+      <c r="O9" s="1" t="n">
+        <v>90.5868189354164</v>
+      </c>
+      <c r="P9" s="1" t="n">
+        <v>37.9035871203964</v>
+      </c>
+      <c r="Q9" s="1" t="n">
+        <v>40.3697283407564</v>
+      </c>
+      <c r="R9" s="1" t="n">
+        <v>39.9689439664092</v>
+      </c>
+      <c r="S9" s="1" t="n">
+        <v>43.7701728738714</v>
+      </c>
+      <c r="T9" s="1" t="n">
+        <v>42.2053190283762</v>
+      </c>
+      <c r="U9" s="1" t="n">
+        <v>42.0504065027361</v>
+      </c>
+      <c r="V9" s="1" t="n">
+        <v>37.5261607005142</v>
+      </c>
+      <c r="W9" s="1" t="n">
+        <v>39.808866914046</v>
+      </c>
+      <c r="X9" s="1" t="n">
+        <v>45.5398127012069</v>
+      </c>
+      <c r="Y9" s="1" t="n">
+        <v>46.5786397293642</v>
+      </c>
+      <c r="Z9" s="1" t="n">
+        <v>48.097119142325</v>
+      </c>
+      <c r="AA9" s="1" t="n">
+        <v>53.9553141671841</v>
+      </c>
+      <c r="AB9" s="1" t="n">
+        <v>56.8369813374168</v>
+      </c>
+      <c r="AC9" s="1" t="n">
+        <v>54.6554031688876</v>
+      </c>
+      <c r="AD9" s="1" t="n">
+        <v>61.413465323765</v>
+      </c>
+      <c r="AE9" s="1" t="n">
+        <v>60.8471218490168</v>
+      </c>
+      <c r="AF9" s="1" t="n">
+        <v>59.4342022837237</v>
+      </c>
+      <c r="AG9" s="1" t="n">
+        <v>65.7441311322412</v>
+      </c>
+      <c r="AH9" s="1" t="n">
+        <v>65.7006020727048</v>
+      </c>
+      <c r="AI9" s="1" t="n">
+        <v>58.7551722408877</v>
+      </c>
+      <c r="AJ9" s="1" t="n">
+        <v>67.4423395605209</v>
+      </c>
+      <c r="AK9" s="1" t="n">
+        <v>66.7123507016619</v>
+      </c>
+      <c r="AL9" s="1" t="n">
+        <v>64.7529097038486</v>
+      </c>
+      <c r="AM9" s="1" t="n">
+        <v>68.6409414477547</v>
+      </c>
+      <c r="AN9" s="1" t="n">
+        <v>69.4477941852617</v>
+      </c>
+      <c r="AO9" s="1" t="n">
+        <v>62.75002964902</v>
+      </c>
+      <c r="AP9" s="1" t="n">
+        <v>70.8835265214945</v>
+      </c>
+      <c r="AQ9" s="1" t="n">
+        <v>68.8070829591896</v>
+      </c>
+      <c r="AR9" s="1" t="n">
+        <v>66.7033339265702</v>
+      </c>
+      <c r="AS9" s="1" t="n">
+        <v>69.3864082779932</v>
+      </c>
+      <c r="AT9" s="1" t="n">
+        <v>71.2090480588324</v>
+      </c>
+      <c r="AU9" s="1" t="n">
+        <v>57.8114923048293</v>
+      </c>
+      <c r="AV9" s="1" t="n">
+        <v>69.0405802588673</v>
+      </c>
+      <c r="AW9" s="1" t="n">
+        <v>63.2856184163346</v>
+      </c>
+      <c r="AX9" s="1" t="n">
+        <v>59.6537582160233</v>
+      </c>
+      <c r="AY9" s="1" t="n">
+        <v>64.4248099193917</v>
+      </c>
+      <c r="AZ9" s="1" t="n">
+        <v>58.3407144214908</v>
+      </c>
+      <c r="BA9" s="1" t="n">
+        <v>59.9017351885839</v>
+      </c>
+      <c r="BB9" s="1" t="n">
+        <v>64.2798615816773</v>
+      </c>
+      <c r="BC9" s="1" t="n">
+        <v>57.7473774551757</v>
+      </c>
+      <c r="BD9" s="1" t="n">
+        <v>81.8962807546129</v>
+      </c>
+      <c r="BE9" s="1" t="n">
+        <v>78.7464238025124</v>
+      </c>
+      <c r="BF9" s="1" t="n">
+        <v>51.4476635509747</v>
+      </c>
+      <c r="BG9" s="1" t="n">
+        <v>105.829983504986</v>
+      </c>
+      <c r="BH9" s="1" t="n">
+        <v>92.62493282292</v>
+      </c>
+      <c r="BI9" s="1" t="n">
+        <v>104.706544881278</v>
+      </c>
+      <c r="BJ9" s="1" t="n">
+        <v>116.594619879365</v>
+      </c>
+      <c r="BK9" s="1" t="n">
+        <v>123.222465241597</v>
+      </c>
+      <c r="BL9" s="1" t="n">
+        <v>94.1918748835307</v>
+      </c>
+      <c r="BM9" s="1" t="n">
+        <v>67.4637300952251</v>
+      </c>
+      <c r="BN9" s="1" t="n">
+        <v>57.3127520671304</v>
+      </c>
+      <c r="BO9" s="1" t="n">
+        <v>87.2534670865509</v>
+      </c>
+      <c r="BP9" s="1" t="n">
+        <v>87.2534670865509</v>
+      </c>
+      <c r="BQ9" s="1" t="n">
+        <v>87.2534670865509</v>
+      </c>
+      <c r="BR9" s="1" t="n">
+        <v>87.2534670865509</v>
+      </c>
+      <c r="BS9" s="1" t="n">
+        <v>106.878670969337</v>
+      </c>
+      <c r="BT9" s="1" t="n">
+        <v>114.333892467344</v>
+      </c>
+      <c r="BU9" s="1" t="n">
+        <v>115.917864399838</v>
+      </c>
+      <c r="BV9" s="1" t="n">
+        <v>2.94770071778572</v>
+      </c>
+      <c r="BW9" s="1" t="n">
+        <v>2.53319750361371E-012</v>
+      </c>
+      <c r="BX9" s="1" t="n">
+        <v>113.148854918083</v>
+      </c>
+      <c r="BY9" s="1" t="n">
+        <v>114.638141046986</v>
+      </c>
+      <c r="BZ9" s="1" t="n">
+        <v>106.247183584898</v>
+      </c>
+      <c r="CA9" s="1" t="n">
+        <v>51.9184704414644</v>
+      </c>
+      <c r="CB9" s="1" t="n">
+        <v>74.1692434878064</v>
+      </c>
+      <c r="CC9" s="1" t="n">
+        <v>74.1692434878064</v>
+      </c>
+      <c r="CD9" s="1" t="n">
+        <v>51.9184704414644</v>
+      </c>
+      <c r="CE9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="CF9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="CG9" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>95.788581013752</v>
+      </c>
+      <c r="E10" s="1" t="n">
+        <v>106.809754938707</v>
+      </c>
+      <c r="F10" s="1" t="n">
+        <v>103.442481380348</v>
+      </c>
+      <c r="G10" s="1" t="n">
+        <v>79.8495933840465</v>
+      </c>
+      <c r="H10" s="1" t="n">
+        <v>99.5261733534472</v>
+      </c>
+      <c r="I10" s="1" t="n">
+        <v>92.6205163866611</v>
+      </c>
+      <c r="J10" s="1" t="n">
+        <v>70.8190173843644</v>
+      </c>
+      <c r="K10" s="1" t="n">
+        <v>94.9975099017104</v>
+      </c>
+      <c r="L10" s="1" t="n">
+        <v>79.1799044258065</v>
+      </c>
+      <c r="M10" s="1" t="n">
+        <v>19.6859344171111</v>
+      </c>
+      <c r="N10" s="1" t="n">
+        <v>81.5119183548589</v>
+      </c>
+      <c r="O10" s="1" t="n">
+        <v>90.5868189354164</v>
+      </c>
+      <c r="P10" s="1" t="n">
+        <v>37.9035871203964</v>
+      </c>
+      <c r="Q10" s="1" t="n">
+        <v>40.3697283407564</v>
+      </c>
+      <c r="R10" s="1" t="n">
+        <v>39.9689439664092</v>
+      </c>
+      <c r="S10" s="1" t="n">
+        <v>43.7701728738714</v>
+      </c>
+      <c r="T10" s="1" t="n">
+        <v>42.2053190283762</v>
+      </c>
+      <c r="U10" s="1" t="n">
+        <v>42.0504065027361</v>
+      </c>
+      <c r="V10" s="1" t="n">
+        <v>37.5261607005142</v>
+      </c>
+      <c r="W10" s="1" t="n">
+        <v>39.808866914046</v>
+      </c>
+      <c r="X10" s="1" t="n">
+        <v>45.5398127012069</v>
+      </c>
+      <c r="Y10" s="1" t="n">
+        <v>46.5786397293642</v>
+      </c>
+      <c r="Z10" s="1" t="n">
+        <v>48.097119142325</v>
+      </c>
+      <c r="AA10" s="1" t="n">
+        <v>53.9553141671841</v>
+      </c>
+      <c r="AB10" s="1" t="n">
+        <v>56.8369813374168</v>
+      </c>
+      <c r="AC10" s="1" t="n">
+        <v>54.6554031688876</v>
+      </c>
+      <c r="AD10" s="1" t="n">
+        <v>61.413465323765</v>
+      </c>
+      <c r="AE10" s="1" t="n">
+        <v>60.8471218490168</v>
+      </c>
+      <c r="AF10" s="1" t="n">
+        <v>59.4342022837237</v>
+      </c>
+      <c r="AG10" s="1" t="n">
+        <v>65.7441311322412</v>
+      </c>
+      <c r="AH10" s="1" t="n">
+        <v>65.7006020727048</v>
+      </c>
+      <c r="AI10" s="1" t="n">
+        <v>58.7551722408877</v>
+      </c>
+      <c r="AJ10" s="1" t="n">
+        <v>67.4423395605209</v>
+      </c>
+      <c r="AK10" s="1" t="n">
+        <v>66.7123507016619</v>
+      </c>
+      <c r="AL10" s="1" t="n">
+        <v>64.7529097038486</v>
+      </c>
+      <c r="AM10" s="1" t="n">
+        <v>68.6409414477547</v>
+      </c>
+      <c r="AN10" s="1" t="n">
+        <v>69.4477941852617</v>
+      </c>
+      <c r="AO10" s="1" t="n">
+        <v>62.75002964902</v>
+      </c>
+      <c r="AP10" s="1" t="n">
+        <v>70.8835265214945</v>
+      </c>
+      <c r="AQ10" s="1" t="n">
+        <v>68.8070829591896</v>
+      </c>
+      <c r="AR10" s="1" t="n">
+        <v>66.7033339265702</v>
+      </c>
+      <c r="AS10" s="1" t="n">
+        <v>69.3864082779932</v>
+      </c>
+      <c r="AT10" s="1" t="n">
+        <v>72.1124906647618</v>
+      </c>
+      <c r="AU10" s="1" t="n">
+        <v>59.6763827875555</v>
+      </c>
+      <c r="AV10" s="1" t="n">
+        <v>72.5756143596382</v>
+      </c>
+      <c r="AW10" s="1" t="n">
+        <v>67.2629552799383</v>
+      </c>
+      <c r="AX10" s="1" t="n">
+        <v>64.4779277908496</v>
+      </c>
+      <c r="AY10" s="1" t="n">
+        <v>70.7628660528634</v>
+      </c>
+      <c r="AZ10" s="1" t="n">
+        <v>64.7099264398374</v>
+      </c>
+      <c r="BA10" s="1" t="n">
+        <v>67.4444354769421</v>
+      </c>
+      <c r="BB10" s="1" t="n">
+        <v>73.0771221030668</v>
+      </c>
+      <c r="BC10" s="1" t="n">
+        <v>65.6547581551492</v>
+      </c>
+      <c r="BD10" s="1" t="n">
+        <v>93.1103842927571</v>
+      </c>
+      <c r="BE10" s="1" t="n">
+        <v>89.5292156661126</v>
+      </c>
+      <c r="BF10" s="1" t="n">
+        <v>58.4924209018602</v>
+      </c>
+      <c r="BG10" s="1" t="n">
+        <v>120.32134234973</v>
+      </c>
+      <c r="BH10" s="1" t="n">
+        <v>105.308116690599</v>
+      </c>
+      <c r="BI10" s="1" t="n">
+        <v>119.044070646804</v>
+      </c>
+      <c r="BJ10" s="1" t="n">
+        <v>132.559986404805</v>
+      </c>
+      <c r="BK10" s="1" t="n">
+        <v>140.095386340237</v>
+      </c>
+      <c r="BL10" s="1" t="n">
+        <v>107.089621004148</v>
+      </c>
+      <c r="BM10" s="1" t="n">
+        <v>76.7015763977222</v>
+      </c>
+      <c r="BN10" s="1" t="n">
+        <v>65.1606192695808</v>
+      </c>
+      <c r="BO10" s="1" t="n">
+        <v>117.722520187916</v>
+      </c>
+      <c r="BP10" s="1" t="n">
+        <v>117.722520187916</v>
+      </c>
+      <c r="BQ10" s="1" t="n">
+        <v>117.722520187916</v>
+      </c>
+      <c r="BR10" s="1" t="n">
+        <v>117.722520187916</v>
+      </c>
+      <c r="BS10" s="1" t="n">
+        <v>121.511988042181</v>
+      </c>
+      <c r="BT10" s="1" t="n">
+        <v>129.98794285432</v>
+      </c>
+      <c r="BU10" s="1" t="n">
+        <v>131.788784657224</v>
+      </c>
+      <c r="BV10" s="1" t="n">
+        <v>3.35128581898503</v>
+      </c>
+      <c r="BW10" s="1" t="n">
+        <v>2.88003080479829E-012</v>
+      </c>
+      <c r="BX10" s="1" t="n">
+        <v>128.640655624705</v>
+      </c>
+      <c r="BY10" s="1" t="n">
+        <v>130.3338476961</v>
+      </c>
+      <c r="BZ10" s="1" t="n">
+        <v>120.794040421661</v>
+      </c>
+      <c r="CA10" s="1" t="n">
+        <v>59.0268994012985</v>
+      </c>
+      <c r="CB10" s="1" t="n">
+        <v>84.3241420018551</v>
+      </c>
+      <c r="CC10" s="1" t="n">
+        <v>84.3241420018551</v>
+      </c>
+      <c r="CD10" s="1" t="n">
+        <v>59.0268994012985</v>
+      </c>
+      <c r="CE10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="CF10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="CG10" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>